<commit_message>
added full_match and teted two sheets in 1 yaml
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -4,19 +4,20 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Example" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Students" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mj5Vg5TQSC9tgukmQ7JlHZq9JGLwA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mhD6SaTNa3FSw3bCTki5U5s2ERxAg=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>ID</t>
   </si>
@@ -121,6 +122,48 @@
   </si>
   <si>
     <t>max34</t>
+  </si>
+  <si>
+    <t>Roll No</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Course</t>
+  </si>
+  <si>
+    <t>Batch</t>
+  </si>
+  <si>
+    <t>MAR2022001</t>
+  </si>
+  <si>
+    <t>Deepak Sharma</t>
+  </si>
+  <si>
+    <t>Mumbai</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>MUM123</t>
+  </si>
+  <si>
+    <t>MAR2022002</t>
+  </si>
+  <si>
+    <t>Deep@k $harma</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>DEL123</t>
   </si>
 </sst>
 </file>
@@ -131,7 +174,7 @@
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -151,6 +194,17 @@
       <u/>
       <sz val="11.0"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11.0"/>
+      <color rgb="FF0563C1"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -180,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -206,6 +260,15 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -215,6 +278,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1583,4 +1650,71 @@
   <pageSetup paperSize="9" orientation="portrait"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="B3"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>